<commit_message>
format color for empty seats
</commit_message>
<xml_diff>
--- a/Temp/Transfer/Seat Map.xlsx
+++ b/Temp/Transfer/Seat Map.xlsx
@@ -464,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -482,14 +482,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -567,7 +561,67 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -869,8 +923,8 @@
   </sheetPr>
   <dimension ref="B1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,128 +942,128 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="26"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="40" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="42"/>
-    </row>
-    <row r="3" spans="2:11" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="28"/>
-      <c r="C3" s="38" t="s">
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="40"/>
+    </row>
+    <row r="3" spans="2:11" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="26"/>
+      <c r="C3" s="36" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="12"/>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="36" t="s">
         <v>42</v>
       </c>
       <c r="F3" s="12"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="45"/>
-    </row>
-    <row r="4" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="28"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="43"/>
+    </row>
+    <row r="4" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="26"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="37" t="s">
+      <c r="I4" s="14"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="35" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="28"/>
+    <row r="5" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="26"/>
       <c r="C5" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="30" t="s">
         <v>41</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="37"/>
-    </row>
-    <row r="6" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="28"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="35"/>
+    </row>
+    <row r="6" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="26"/>
       <c r="C6" s="12"/>
-      <c r="D6" s="17"/>
+      <c r="D6" s="15"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="37"/>
-    </row>
-    <row r="7" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="28"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="35"/>
+    </row>
+    <row r="7" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="26"/>
       <c r="C7" s="11" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="19"/>
-    </row>
-    <row r="8" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="28"/>
-      <c r="C8" s="14" t="s">
+      <c r="I7" s="14"/>
+      <c r="J7" s="17"/>
+    </row>
+    <row r="8" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="26"/>
+      <c r="C8" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>3</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="16"/>
-      <c r="J8" s="19"/>
-    </row>
-    <row r="9" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="28"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="17"/>
+    </row>
+    <row r="9" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="26"/>
       <c r="C9" s="12"/>
-      <c r="D9" s="17"/>
+      <c r="D9" s="15"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="19"/>
-    </row>
-    <row r="10" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="28"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="17"/>
+    </row>
+    <row r="10" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="26"/>
       <c r="C10" s="12"/>
       <c r="D10" s="11" t="s">
         <v>39</v>
@@ -1018,57 +1072,57 @@
         <v>40</v>
       </c>
       <c r="F10" s="12"/>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="35" t="s">
+      <c r="I10" s="14"/>
+      <c r="J10" s="33" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="28"/>
+    <row r="11" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="26"/>
       <c r="C11" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="12"/>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="I11" s="16"/>
-      <c r="J11" s="35" t="s">
+      <c r="I11" s="14"/>
+      <c r="J11" s="33" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="28"/>
+    <row r="12" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="26"/>
       <c r="C12" s="12"/>
-      <c r="D12" s="17"/>
+      <c r="D12" s="15"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="19"/>
-    </row>
-    <row r="13" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="28"/>
-      <c r="C13" s="14" t="s">
+      <c r="I12" s="14"/>
+      <c r="J12" s="17"/>
+    </row>
+    <row r="13" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="26"/>
+      <c r="C13" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>34</v>
       </c>
       <c r="E13" s="11" t="s">
@@ -1081,14 +1135,14 @@
       <c r="H13" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="15" t="s">
+      <c r="I13" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="J13" s="19"/>
-    </row>
-    <row r="14" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="28"/>
-      <c r="C14" s="14" t="s">
+      <c r="J13" s="17"/>
+    </row>
+    <row r="14" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="26"/>
+      <c r="C14" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="11" t="s">
@@ -1101,29 +1155,29 @@
       <c r="G14" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="15"/>
-      <c r="J14" s="19"/>
-    </row>
-    <row r="15" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="28"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="17"/>
+    </row>
+    <row r="15" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="26"/>
       <c r="C15" s="12"/>
-      <c r="D15" s="17"/>
+      <c r="D15" s="15"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="19"/>
-    </row>
-    <row r="16" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="28"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="17"/>
+    </row>
+    <row r="16" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="26"/>
       <c r="C16" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="13" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="11" t="s">
@@ -1136,17 +1190,17 @@
       <c r="H16" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="15" t="s">
+      <c r="I16" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="J16" s="19"/>
-    </row>
-    <row r="17" spans="2:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="28"/>
+      <c r="J16" s="17"/>
+    </row>
+    <row r="17" spans="2:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="26"/>
       <c r="C17" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="13" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="11" t="s">
@@ -1159,19 +1213,19 @@
       <c r="H17" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="15"/>
-      <c r="J17" s="19"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="17"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="29"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="21"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="19"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -1181,6 +1235,11 @@
     <mergeCell ref="I16:I17"/>
     <mergeCell ref="G2:J3"/>
   </mergeCells>
+  <conditionalFormatting sqref="C5:I17">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Empty"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="53" orientation="landscape" r:id="rId1"/>
 </worksheet>
@@ -1193,8 +1252,8 @@
   </sheetPr>
   <dimension ref="B2:V21"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:J5"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,281 +1281,281 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="M2" s="39" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="M2" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
     </row>
     <row r="3" spans="2:22" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="24"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
     </row>
     <row r="4" spans="2:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="40" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="42"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="40" t="s">
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="40"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="S4" s="41"/>
-      <c r="T4" s="41"/>
-      <c r="U4" s="42"/>
+      <c r="S4" s="39"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="40"/>
     </row>
     <row r="5" spans="2:22" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="28"/>
-      <c r="C5" s="38" t="s">
+      <c r="B5" s="26"/>
+      <c r="C5" s="36" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="12"/>
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="36" t="s">
         <v>42</v>
       </c>
       <c r="F5" s="12"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="45"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="38" t="s">
+      <c r="G5" s="41"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="43"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="36" t="s">
         <v>24</v>
       </c>
       <c r="O5" s="12"/>
-      <c r="P5" s="38" t="s">
+      <c r="P5" s="36" t="s">
         <v>42</v>
       </c>
       <c r="Q5" s="12"/>
-      <c r="R5" s="43"/>
-      <c r="S5" s="44"/>
-      <c r="T5" s="44"/>
-      <c r="U5" s="45"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="42"/>
+      <c r="U5" s="43"/>
     </row>
     <row r="6" spans="2:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="28"/>
+      <c r="B6" s="26"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="36" t="s">
+      <c r="I6" s="14"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="L6" s="23"/>
-      <c r="M6" s="28"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="26"/>
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
       <c r="Q6" s="12"/>
       <c r="R6" s="12"/>
       <c r="S6" s="12"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="22"/>
-      <c r="V6" s="36" t="s">
+      <c r="T6" s="14"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="34" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="2:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="28"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="30" t="s">
         <v>41</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="28"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="26"/>
       <c r="N7" s="11" t="s">
         <v>2</v>
       </c>
       <c r="O7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="P7" s="13" t="s">
+      <c r="P7" s="30" t="s">
         <v>41</v>
       </c>
       <c r="Q7" s="12"/>
       <c r="R7" s="12"/>
       <c r="S7" s="12"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="22"/>
-      <c r="V7" s="36"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="34"/>
     </row>
     <row r="8" spans="2:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="28"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="12"/>
-      <c r="D8" s="17"/>
+      <c r="D8" s="15"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="28"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="26"/>
       <c r="N8" s="12"/>
-      <c r="O8" s="17"/>
+      <c r="O8" s="15"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="12"/>
       <c r="R8" s="12"/>
       <c r="S8" s="12"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="22"/>
-      <c r="V8" s="36"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="20"/>
+      <c r="V8" s="34"/>
     </row>
     <row r="9" spans="2:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="28"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>29</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="19"/>
-      <c r="M9" s="28"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="17"/>
+      <c r="M9" s="26"/>
       <c r="N9" s="11" t="s">
         <v>32</v>
       </c>
       <c r="O9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="P9" s="14" t="s">
+      <c r="P9" s="13" t="s">
         <v>15</v>
       </c>
       <c r="Q9" s="12"/>
       <c r="R9" s="12"/>
       <c r="S9" s="12"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="19"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="17"/>
     </row>
     <row r="10" spans="2:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="28"/>
-      <c r="C10" s="14" t="s">
+      <c r="B10" s="26"/>
+      <c r="C10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="19"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="14" t="s">
+      <c r="I10" s="14"/>
+      <c r="J10" s="17"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="O10" s="14" t="s">
+      <c r="O10" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="P10" s="14" t="s">
+      <c r="P10" s="13" t="s">
         <v>3</v>
       </c>
       <c r="Q10" s="12"/>
       <c r="R10" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="S10" s="14" t="s">
+      <c r="S10" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="T10" s="16"/>
-      <c r="U10" s="19"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="17"/>
     </row>
     <row r="11" spans="2:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="28"/>
+      <c r="B11" s="26"/>
       <c r="C11" s="12"/>
-      <c r="D11" s="17"/>
+      <c r="D11" s="15"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="19"/>
-      <c r="M11" s="28"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="17"/>
+      <c r="M11" s="26"/>
       <c r="N11" s="12"/>
-      <c r="O11" s="17"/>
+      <c r="O11" s="15"/>
       <c r="P11" s="12"/>
       <c r="Q11" s="12"/>
       <c r="R11" s="12"/>
       <c r="S11" s="12"/>
-      <c r="T11" s="16"/>
-      <c r="U11" s="19"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="17"/>
     </row>
     <row r="12" spans="2:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="28"/>
+      <c r="B12" s="26"/>
       <c r="C12" s="12"/>
       <c r="D12" s="11" t="s">
         <v>4</v>
@@ -1505,17 +1564,17 @@
         <v>30</v>
       </c>
       <c r="F12" s="12"/>
-      <c r="G12" s="32" t="s">
+      <c r="G12" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="32" t="s">
+      <c r="H12" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="16"/>
-      <c r="J12" s="20" t="s">
+      <c r="I12" s="14"/>
+      <c r="J12" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="M12" s="28"/>
+      <c r="M12" s="26"/>
       <c r="N12" s="12"/>
       <c r="O12" s="11" t="s">
         <v>39</v>
@@ -1524,87 +1583,87 @@
         <v>40</v>
       </c>
       <c r="Q12" s="12"/>
-      <c r="R12" s="13" t="s">
+      <c r="R12" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="S12" s="13" t="s">
+      <c r="S12" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="T12" s="16"/>
-      <c r="U12" s="20" t="s">
+      <c r="T12" s="14"/>
+      <c r="U12" s="18" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="13" spans="2:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="28"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="13" t="s">
         <v>3</v>
       </c>
       <c r="F13" s="12"/>
-      <c r="G13" s="32" t="s">
+      <c r="G13" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="32" t="s">
+      <c r="H13" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="16"/>
-      <c r="J13" s="20" t="s">
+      <c r="I13" s="14"/>
+      <c r="J13" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="M13" s="28"/>
+      <c r="M13" s="26"/>
       <c r="N13" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="O13" s="14" t="s">
+      <c r="O13" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="P13" s="14" t="s">
+      <c r="P13" s="13" t="s">
         <v>7</v>
       </c>
       <c r="Q13" s="12"/>
-      <c r="R13" s="13" t="s">
+      <c r="R13" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="S13" s="13" t="s">
+      <c r="S13" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="T13" s="16"/>
-      <c r="U13" s="20" t="s">
+      <c r="T13" s="14"/>
+      <c r="U13" s="18" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="14" spans="2:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="28"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="12"/>
-      <c r="D14" s="17"/>
+      <c r="D14" s="15"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="19"/>
-      <c r="M14" s="28"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="17"/>
+      <c r="M14" s="26"/>
       <c r="N14" s="12"/>
-      <c r="O14" s="17"/>
+      <c r="O14" s="15"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
       <c r="R14" s="12"/>
       <c r="S14" s="12"/>
-      <c r="T14" s="16"/>
-      <c r="U14" s="19"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="17"/>
     </row>
     <row r="15" spans="2:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="28"/>
-      <c r="C15" s="14" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="13" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="11" t="s">
@@ -1617,15 +1676,15 @@
       <c r="H15" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="15" t="s">
+      <c r="I15" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="J15" s="19"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="14" t="s">
+      <c r="J15" s="17"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="O15" s="14" t="s">
+      <c r="O15" s="13" t="s">
         <v>34</v>
       </c>
       <c r="P15" s="11" t="s">
@@ -1638,14 +1697,14 @@
       <c r="S15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="T15" s="15" t="s">
+      <c r="T15" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="U15" s="19"/>
+      <c r="U15" s="17"/>
     </row>
     <row r="16" spans="2:22" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="28"/>
-      <c r="C16" s="14" t="s">
+      <c r="B16" s="26"/>
+      <c r="C16" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="11" t="s">
@@ -1658,13 +1717,13 @@
       <c r="G16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H16" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="15"/>
-      <c r="J16" s="19"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="14" t="s">
+      <c r="I16" s="31"/>
+      <c r="J16" s="17"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="13" t="s">
         <v>5</v>
       </c>
       <c r="O16" s="11" t="s">
@@ -1677,36 +1736,36 @@
       <c r="R16" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="S16" s="14" t="s">
+      <c r="S16" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="T16" s="15"/>
-      <c r="U16" s="19"/>
+      <c r="T16" s="31"/>
+      <c r="U16" s="17"/>
     </row>
     <row r="17" spans="2:21" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="28"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="12"/>
-      <c r="D17" s="17"/>
+      <c r="D17" s="15"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="19"/>
-      <c r="M17" s="28"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="17"/>
+      <c r="M17" s="26"/>
       <c r="N17" s="12"/>
-      <c r="O17" s="17"/>
+      <c r="O17" s="15"/>
       <c r="P17" s="12"/>
       <c r="Q17" s="12"/>
       <c r="R17" s="12"/>
       <c r="S17" s="12"/>
-      <c r="T17" s="16"/>
-      <c r="U17" s="19"/>
+      <c r="T17" s="14"/>
+      <c r="U17" s="17"/>
     </row>
     <row r="18" spans="2:21" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="28"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="12"/>
-      <c r="D18" s="34"/>
+      <c r="D18" s="32"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="11" t="s">
@@ -1715,15 +1774,15 @@
       <c r="H18" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="33" t="s">
+      <c r="I18" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="19"/>
-      <c r="M18" s="28"/>
+      <c r="J18" s="17"/>
+      <c r="M18" s="26"/>
       <c r="N18" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="O18" s="14" t="s">
+      <c r="O18" s="13" t="s">
         <v>11</v>
       </c>
       <c r="P18" s="11" t="s">
@@ -1736,15 +1795,15 @@
       <c r="S18" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="T18" s="15" t="s">
+      <c r="T18" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="U18" s="19"/>
+      <c r="U18" s="17"/>
     </row>
     <row r="19" spans="2:21" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="28"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="12"/>
-      <c r="D19" s="34"/>
+      <c r="D19" s="32"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
       <c r="G19" s="11" t="s">
@@ -1753,13 +1812,13 @@
       <c r="H19" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="33"/>
-      <c r="J19" s="19"/>
-      <c r="M19" s="28"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="17"/>
+      <c r="M19" s="26"/>
       <c r="N19" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="O19" s="14" t="s">
+      <c r="O19" s="13" t="s">
         <v>9</v>
       </c>
       <c r="P19" s="11" t="s">
@@ -1772,28 +1831,28 @@
       <c r="S19" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="T19" s="15"/>
-      <c r="U19" s="19"/>
+      <c r="T19" s="31"/>
+      <c r="U19" s="17"/>
     </row>
     <row r="20" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="29"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="21"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="31"/>
-      <c r="P20" s="30"/>
-      <c r="Q20" s="30"/>
-      <c r="R20" s="30"/>
-      <c r="S20" s="30"/>
-      <c r="T20" s="30"/>
-      <c r="U20" s="21"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="19"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="28"/>
+      <c r="R20" s="28"/>
+      <c r="S20" s="28"/>
+      <c r="T20" s="28"/>
+      <c r="U20" s="19"/>
     </row>
     <row r="21" spans="2:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -1809,6 +1868,16 @@
     <mergeCell ref="T15:T16"/>
     <mergeCell ref="T18:T19"/>
   </mergeCells>
+  <conditionalFormatting sqref="C7:I19">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>"Empty"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N7:T19">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Empty"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="53" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>